<commit_message>
I didnt check if passif and actif are correct
</commit_message>
<xml_diff>
--- a/data/transcriptions/IMG_2024_03_19_12_00_56_579.xlsx
+++ b/data/transcriptions/IMG_2024_03_19_12_00_56_579.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\julie\Documents\GitHub\img-analysis_seorin_project\data\transcriptions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{656AA145-900C-42E7-8347-7ED8676E4B68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10B1438D-2B05-4A31-AE33-93986825B1B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{6D6EFBF4-D3F9-A04D-9AC4-202B897D114E}"/>
   </bookViews>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="69">
   <si>
     <t>Nom.</t>
   </si>
@@ -135,6 +135,176 @@
   </si>
   <si>
     <t>N' d'ordre</t>
+  </si>
+  <si>
+    <t>Arrété le seize juin 1921 servais</t>
+  </si>
+  <si>
+    <t>Suyex</t>
+  </si>
+  <si>
+    <t>Arrété le dix sept juin 1921 servais</t>
+  </si>
+  <si>
+    <t>Masson</t>
+  </si>
+  <si>
+    <t>Arrété le dix huit juin 1921 servais</t>
+  </si>
+  <si>
+    <t>Arrété le vingt juin 1921 servais</t>
+  </si>
+  <si>
+    <t>Arrété le dix neuf juin 1921 Dimanche servais</t>
+  </si>
+  <si>
+    <t>Seblicq</t>
+  </si>
+  <si>
+    <t>Arrété le ving un juin 1921 servais</t>
+  </si>
+  <si>
+    <t>Arrété le ving deux juin 1921 servais</t>
+  </si>
+  <si>
+    <t>Arrété le ving trois juin 1921 servais</t>
+  </si>
+  <si>
+    <t>Dasset</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>Kegelart</t>
+  </si>
+  <si>
+    <t>dix sept juin</t>
+  </si>
+  <si>
+    <t>dix huit juin</t>
+  </si>
+  <si>
+    <t>vingt un juin</t>
+  </si>
+  <si>
+    <t>ving quatre</t>
+  </si>
+  <si>
+    <t>Charles Louis</t>
+  </si>
+  <si>
+    <t>Jean Baptiste</t>
+  </si>
+  <si>
+    <t>Emmanuel Joseph</t>
+  </si>
+  <si>
+    <t>Laurent Joseph</t>
+  </si>
+  <si>
+    <t>Virginal</t>
+  </si>
+  <si>
+    <t>Baulers</t>
+  </si>
+  <si>
+    <t>Quenast</t>
+  </si>
+  <si>
+    <t>Braine-l'Alleud</t>
+  </si>
+  <si>
+    <t>16 novembre 1920</t>
+  </si>
+  <si>
+    <t>19 décembre 1920</t>
+  </si>
+  <si>
+    <t>13 mars 1920</t>
+  </si>
+  <si>
+    <t>30 juillet 1920</t>
+  </si>
+  <si>
+    <t>29 mai 1920</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Van </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>…</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Julienne &amp; autres</t>
+    </r>
+  </si>
+  <si>
+    <t>Rose Eloise</t>
+  </si>
+  <si>
+    <r>
+      <t>Pierot</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Marie Obirèle</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> &amp; autres</t>
+    </r>
+  </si>
+  <si>
+    <t>Giriss Emilie &amp; autres</t>
+  </si>
+  <si>
+    <t>Hazart Elisabeth &amp; autres</t>
+  </si>
+  <si>
+    <t>260(5)/1922</t>
+  </si>
+  <si>
+    <t>non passible</t>
+  </si>
+  <si>
+    <t>28 novembre 1921</t>
+  </si>
+  <si>
+    <t>16 septembre 1921</t>
+  </si>
+  <si>
+    <t>28 - 11 - 1921</t>
+  </si>
+  <si>
+    <t>4 janvier 1922</t>
   </si>
 </sst>
 </file>
@@ -170,12 +340,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="13">
@@ -328,7 +504,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
@@ -368,8 +544,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -718,10 +893,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB076F5B-4564-1543-8968-7E29FE54F40E}">
-  <dimension ref="A1:U20"/>
+  <dimension ref="A1:U21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="72" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="R11" sqref="R11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -836,8 +1011,11 @@
     <row r="3" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A3" s="3"/>
       <c r="B3" s="1"/>
+      <c r="C3" t="s">
+        <v>27</v>
+      </c>
       <c r="F3" s="1"/>
-      <c r="G3" s="2"/>
+      <c r="G3" s="19"/>
       <c r="H3" s="2"/>
       <c r="K3" s="1"/>
       <c r="L3" s="2"/>
@@ -851,44 +1029,83 @@
       <c r="U3" s="2"/>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A4" s="3"/>
-      <c r="B4" s="15"/>
-      <c r="E4" s="11"/>
+      <c r="A4" s="3">
+        <v>145</v>
+      </c>
+      <c r="B4" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="D4" t="s">
+        <v>45</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>49</v>
+      </c>
       <c r="F4" s="16"/>
-      <c r="G4" s="16"/>
-      <c r="H4" s="2"/>
-      <c r="K4" s="14"/>
+      <c r="G4" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="I4">
+        <v>54845</v>
+      </c>
+      <c r="J4">
+        <v>1413</v>
+      </c>
+      <c r="K4" s="15">
+        <v>53432</v>
+      </c>
       <c r="L4" s="2"/>
       <c r="M4" s="13"/>
       <c r="N4" s="1"/>
       <c r="P4" s="1"/>
       <c r="Q4" s="2"/>
-      <c r="R4" s="17"/>
+      <c r="R4" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="S4">
+        <v>174</v>
+      </c>
       <c r="T4" s="2"/>
       <c r="U4" s="2"/>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A5" s="3"/>
-      <c r="B5" s="1"/>
+      <c r="B5" s="15"/>
+      <c r="C5" s="13"/>
       <c r="E5" s="11"/>
       <c r="F5" s="16"/>
       <c r="G5" s="16"/>
       <c r="H5" s="2"/>
-      <c r="K5" s="1"/>
+      <c r="K5" s="15"/>
       <c r="L5" s="2"/>
+      <c r="M5" s="13"/>
       <c r="N5" s="1"/>
       <c r="P5" s="1"/>
       <c r="Q5" s="2"/>
-      <c r="R5" s="17"/>
+      <c r="R5" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="S5">
+        <v>391</v>
+      </c>
       <c r="T5" s="2"/>
       <c r="U5" s="2"/>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A6" s="3"/>
       <c r="B6" s="1"/>
+      <c r="C6" t="s">
+        <v>29</v>
+      </c>
       <c r="E6" s="11"/>
-      <c r="F6" s="17"/>
-      <c r="G6" s="17"/>
+      <c r="F6" s="16"/>
+      <c r="G6" s="16"/>
       <c r="H6" s="2"/>
       <c r="K6" s="1"/>
       <c r="L6" s="2"/>
@@ -900,28 +1117,61 @@
       <c r="U6" s="2"/>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A7" s="3"/>
-      <c r="B7" s="1"/>
+      <c r="A7" s="3">
+        <v>146</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C7" t="s">
+        <v>30</v>
+      </c>
+      <c r="D7" t="s">
+        <v>46</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>50</v>
+      </c>
       <c r="F7" s="17"/>
-      <c r="G7" s="17"/>
-      <c r="H7" s="2"/>
-      <c r="I7" s="13"/>
-      <c r="K7" s="14"/>
+      <c r="G7" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="I7" s="13">
+        <v>12905</v>
+      </c>
+      <c r="J7" s="13">
+        <v>854</v>
+      </c>
+      <c r="K7" s="1">
+        <v>12020</v>
+      </c>
       <c r="L7" s="2"/>
       <c r="N7" s="1"/>
       <c r="P7" s="1"/>
       <c r="Q7" s="2"/>
-      <c r="S7" s="1"/>
+      <c r="R7" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="S7" s="13">
+        <v>169</v>
+      </c>
       <c r="T7" s="2"/>
       <c r="U7" s="2"/>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A8" s="3"/>
       <c r="B8" s="1"/>
-      <c r="F8" s="16"/>
-      <c r="G8" s="16"/>
-      <c r="H8" s="27"/>
-      <c r="K8" s="1"/>
+      <c r="C8" t="s">
+        <v>31</v>
+      </c>
+      <c r="F8" s="17"/>
+      <c r="G8" s="17"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="13"/>
+      <c r="K8" s="14"/>
       <c r="L8" s="2"/>
       <c r="N8" s="1"/>
       <c r="P8" s="1"/>
@@ -933,15 +1183,17 @@
     <row r="9" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A9" s="3"/>
       <c r="B9" s="1"/>
+      <c r="C9" t="s">
+        <v>33</v>
+      </c>
       <c r="F9" s="16"/>
-      <c r="G9" s="2"/>
+      <c r="G9" s="16"/>
       <c r="H9" s="2"/>
       <c r="K9" s="1"/>
       <c r="L9" s="2"/>
       <c r="N9" s="1"/>
       <c r="P9" s="1"/>
       <c r="Q9" s="2"/>
-      <c r="R9" s="17"/>
       <c r="S9" s="1"/>
       <c r="T9" s="2"/>
       <c r="U9" s="2"/>
@@ -949,6 +1201,9 @@
     <row r="10" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A10" s="3"/>
       <c r="B10" s="1"/>
+      <c r="C10" t="s">
+        <v>32</v>
+      </c>
       <c r="F10" s="16"/>
       <c r="G10" s="19"/>
       <c r="H10" s="2"/>
@@ -963,18 +1218,42 @@
       <c r="U10" s="2"/>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A11" s="3"/>
-      <c r="B11" s="1"/>
+      <c r="A11" s="3">
+        <v>147</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C11" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="D11" t="s">
+        <v>46</v>
+      </c>
+      <c r="E11" s="27"/>
       <c r="F11" s="16"/>
-      <c r="G11" s="19"/>
-      <c r="H11" s="2"/>
-      <c r="I11" s="13"/>
-      <c r="K11" s="1"/>
+      <c r="G11" s="19" t="s">
+        <v>55</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="I11">
+        <v>1960</v>
+      </c>
+      <c r="J11">
+        <v>336</v>
+      </c>
+      <c r="K11" s="1">
+        <v>1624</v>
+      </c>
       <c r="L11" s="2"/>
       <c r="N11" s="1"/>
       <c r="P11" s="1"/>
       <c r="Q11" s="2"/>
-      <c r="R11" s="17"/>
+      <c r="R11" t="s">
+        <v>64</v>
+      </c>
       <c r="S11" s="1"/>
       <c r="T11" s="2"/>
       <c r="U11" s="2"/>
@@ -982,9 +1261,13 @@
     <row r="12" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A12" s="3"/>
       <c r="B12" s="1"/>
+      <c r="C12" t="s">
+        <v>35</v>
+      </c>
       <c r="F12" s="16"/>
       <c r="G12" s="19"/>
-      <c r="H12" s="12"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="13"/>
       <c r="K12" s="1"/>
       <c r="L12" s="2"/>
       <c r="N12" s="1"/>
@@ -998,9 +1281,12 @@
     <row r="13" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A13" s="3"/>
       <c r="B13" s="1"/>
+      <c r="C13" t="s">
+        <v>36</v>
+      </c>
       <c r="F13" s="16"/>
-      <c r="G13" s="16"/>
-      <c r="H13" s="2"/>
+      <c r="G13" s="19"/>
+      <c r="H13" s="12"/>
       <c r="K13" s="1"/>
       <c r="L13" s="2"/>
       <c r="N13" s="1"/>
@@ -1014,48 +1300,108 @@
     <row r="14" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A14" s="3"/>
       <c r="B14" s="1"/>
-      <c r="D14" s="28"/>
+      <c r="C14" t="s">
+        <v>37</v>
+      </c>
       <c r="F14" s="16"/>
-      <c r="G14" s="19"/>
+      <c r="G14" s="16"/>
       <c r="H14" s="2"/>
+      <c r="K14" s="1"/>
       <c r="L14" s="2"/>
       <c r="N14" s="1"/>
       <c r="P14" s="1"/>
       <c r="Q14" s="2"/>
+      <c r="R14" s="17"/>
       <c r="S14" s="1"/>
       <c r="T14" s="2"/>
       <c r="U14" s="2"/>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A15" s="3"/>
-      <c r="B15" s="1"/>
+      <c r="A15" s="3">
+        <v>148</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C15" t="s">
+        <v>38</v>
+      </c>
+      <c r="D15" t="s">
+        <v>47</v>
+      </c>
+      <c r="E15" t="s">
+        <v>51</v>
+      </c>
       <c r="F15" s="16"/>
-      <c r="G15" s="19"/>
-      <c r="H15" s="2"/>
+      <c r="G15" s="19" t="s">
+        <v>56</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="I15">
+        <v>2945</v>
+      </c>
+      <c r="J15">
+        <v>1333</v>
+      </c>
+      <c r="K15">
+        <v>1612</v>
+      </c>
       <c r="L15" s="2"/>
-      <c r="N15" s="1"/>
+      <c r="N15" s="1" t="s">
+        <v>63</v>
+      </c>
       <c r="P15" s="1"/>
       <c r="Q15" s="2"/>
-      <c r="R15" s="17"/>
-      <c r="S15" s="1"/>
+      <c r="R15" s="17" t="s">
+        <v>68</v>
+      </c>
+      <c r="S15" s="1">
+        <v>287</v>
+      </c>
       <c r="T15" s="2"/>
       <c r="U15" s="2"/>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A16" s="3"/>
-      <c r="B16" s="1"/>
-      <c r="E16" s="21"/>
+      <c r="A16" s="3">
+        <v>149</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C16" t="s">
+        <v>40</v>
+      </c>
+      <c r="D16" t="s">
+        <v>48</v>
+      </c>
+      <c r="E16" t="s">
+        <v>52</v>
+      </c>
       <c r="F16" s="16"/>
-      <c r="G16" s="19"/>
-      <c r="H16" s="2"/>
-      <c r="I16" s="13"/>
-      <c r="J16" s="13"/>
-      <c r="K16" s="1"/>
+      <c r="G16" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="I16">
+        <v>9836</v>
+      </c>
+      <c r="J16">
+        <v>325</v>
+      </c>
+      <c r="K16">
+        <v>9511</v>
+      </c>
       <c r="L16" s="2"/>
       <c r="N16" s="1"/>
       <c r="P16" s="1"/>
       <c r="Q16" s="2"/>
-      <c r="R16" s="17"/>
+      <c r="R16" t="s">
+        <v>64</v>
+      </c>
       <c r="S16" s="1"/>
       <c r="T16" s="2"/>
       <c r="U16" s="2"/>
@@ -1063,16 +1409,19 @@
     <row r="17" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A17" s="3"/>
       <c r="B17" s="1"/>
+      <c r="E17" s="21"/>
       <c r="F17" s="16"/>
       <c r="G17" s="19"/>
       <c r="H17" s="2"/>
+      <c r="I17" s="13"/>
+      <c r="J17" s="13"/>
       <c r="K17" s="1"/>
       <c r="L17" s="2"/>
       <c r="N17" s="1"/>
       <c r="P17" s="1"/>
       <c r="Q17" s="2"/>
       <c r="R17" s="17"/>
-      <c r="S17" s="14"/>
+      <c r="S17" s="1"/>
       <c r="T17" s="2"/>
       <c r="U17" s="2"/>
     </row>
@@ -1080,7 +1429,7 @@
       <c r="A18" s="3"/>
       <c r="B18" s="1"/>
       <c r="F18" s="16"/>
-      <c r="G18" s="17"/>
+      <c r="G18" s="19"/>
       <c r="H18" s="2"/>
       <c r="K18" s="1"/>
       <c r="L18" s="2"/>
@@ -1088,14 +1437,15 @@
       <c r="P18" s="1"/>
       <c r="Q18" s="2"/>
       <c r="R18" s="17"/>
-      <c r="S18" s="1"/>
+      <c r="S18" s="14"/>
       <c r="T18" s="2"/>
       <c r="U18" s="2"/>
     </row>
     <row r="19" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A19" s="3"/>
       <c r="B19" s="1"/>
       <c r="F19" s="16"/>
-      <c r="G19" s="2"/>
+      <c r="G19" s="17"/>
       <c r="H19" s="2"/>
       <c r="K19" s="1"/>
       <c r="L19" s="2"/>
@@ -1108,27 +1458,42 @@
       <c r="U19" s="2"/>
     </row>
     <row r="20" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A20" s="4"/>
-      <c r="B20" s="5"/>
-      <c r="C20" s="6"/>
-      <c r="D20" s="6"/>
-      <c r="E20" s="6"/>
-      <c r="F20" s="18"/>
-      <c r="G20" s="7"/>
-      <c r="H20" s="7"/>
-      <c r="I20" s="6"/>
-      <c r="J20" s="6"/>
-      <c r="K20" s="5"/>
-      <c r="L20" s="7"/>
-      <c r="M20" s="6"/>
-      <c r="N20" s="5"/>
-      <c r="O20" s="6"/>
-      <c r="P20" s="5"/>
-      <c r="Q20" s="7"/>
-      <c r="R20" s="20"/>
-      <c r="S20" s="5"/>
-      <c r="T20" s="7"/>
-      <c r="U20" s="7"/>
+      <c r="B20" s="1"/>
+      <c r="F20" s="16"/>
+      <c r="G20" s="2"/>
+      <c r="H20" s="2"/>
+      <c r="K20" s="1"/>
+      <c r="L20" s="2"/>
+      <c r="N20" s="1"/>
+      <c r="P20" s="1"/>
+      <c r="Q20" s="2"/>
+      <c r="R20" s="17"/>
+      <c r="S20" s="1"/>
+      <c r="T20" s="2"/>
+      <c r="U20" s="2"/>
+    </row>
+    <row r="21" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A21" s="4"/>
+      <c r="B21" s="5"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="18"/>
+      <c r="G21" s="7"/>
+      <c r="H21" s="7"/>
+      <c r="I21" s="6"/>
+      <c r="J21" s="6"/>
+      <c r="K21" s="5"/>
+      <c r="L21" s="7"/>
+      <c r="M21" s="6"/>
+      <c r="N21" s="5"/>
+      <c r="O21" s="6"/>
+      <c r="P21" s="5"/>
+      <c r="Q21" s="7"/>
+      <c r="R21" s="20"/>
+      <c r="S21" s="5"/>
+      <c r="T21" s="7"/>
+      <c r="U21" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="10">

</xml_diff>